<commit_message>
New results for scaling and imputation methods
</commit_message>
<xml_diff>
--- a/figs/results.xlsx
+++ b/figs/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="2925" tabRatio="503" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="1050" tabRatio="503" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="67">
   <si>
     <t xml:space="preserve">Kullu </t>
   </si>
@@ -183,9 +183,6 @@
     <t>1206-093231</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -217,6 +214,15 @@
   </si>
   <si>
     <t>1206-131028</t>
+  </si>
+  <si>
+    <t>1206-215716</t>
+  </si>
+  <si>
+    <t>1207-181913</t>
+  </si>
+  <si>
+    <t>1208-100402</t>
   </si>
 </sst>
 </file>
@@ -277,7 +283,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -472,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -550,13 +555,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -570,6 +613,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,16 +647,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -613,22 +674,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,36 +689,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1111,10 +1147,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="72"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
@@ -1146,17 +1182,17 @@
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="72" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="72">
         <f>E3+E4</f>
         <v>6548</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="73">
         <f>F3+F4</f>
         <v>0.47360000000000002</v>
       </c>
@@ -1169,12 +1205,12 @@
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="72"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="49"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
       <c r="E4" s="2">
         <v>6548</v>
       </c>
@@ -1184,10 +1220,10 @@
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="2">
         <f>E5</f>
         <v>7277</v>
@@ -1204,74 +1240,74 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="47" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47" t="s">
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47" t="s">
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47" t="s">
+      <c r="B10" s="72"/>
+      <c r="C10" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47" t="s">
+      <c r="D10" s="72"/>
+      <c r="E10" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47" t="s">
+      <c r="F10" s="72"/>
+      <c r="G10" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47" t="s">
+      <c r="H10" s="72"/>
+      <c r="I10" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47" t="s">
+      <c r="J10" s="72"/>
+      <c r="K10" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47" t="s">
+      <c r="L10" s="72"/>
+      <c r="M10" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="47"/>
+      <c r="N10" s="72"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="72" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="72">
         <f>D11+D12</f>
         <v>6548</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="73">
         <f>F11+F12</f>
         <v>0.47363471971066906</v>
       </c>
@@ -1279,14 +1315,14 @@
         <f>D11/(C$11+C$13)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="72">
         <f>H11+H12</f>
         <v>1198</v>
       </c>
       <c r="H11" s="2">
         <v>500</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="73">
         <f>J11+J12</f>
         <v>0.60966921119592876</v>
       </c>
@@ -1294,14 +1330,14 @@
         <f>H11/(G$11+G$13)</f>
         <v>0.2544529262086514</v>
       </c>
-      <c r="K11" s="47">
+      <c r="K11" s="72">
         <f>L11+L12</f>
         <v>4642</v>
       </c>
       <c r="L11" s="2">
         <v>2530</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="73">
         <f>N11+N12</f>
         <v>0.4795454545454545</v>
       </c>
@@ -1311,43 +1347,43 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="2">
         <v>6548</v>
       </c>
-      <c r="E12" s="49"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="6">
         <f t="shared" ref="F12:F13" si="0">D12/(C$11+C$13)</f>
         <v>0.47363471971066906</v>
       </c>
-      <c r="G12" s="47"/>
+      <c r="G12" s="72"/>
       <c r="H12" s="2">
         <v>698</v>
       </c>
-      <c r="I12" s="49"/>
+      <c r="I12" s="73"/>
       <c r="J12" s="6">
         <f t="shared" ref="J12:J13" si="1">H12/(G$11+G$13)</f>
         <v>0.35521628498727736</v>
       </c>
-      <c r="K12" s="47"/>
+      <c r="K12" s="72"/>
       <c r="L12" s="2">
         <v>2112</v>
       </c>
-      <c r="M12" s="49"/>
+      <c r="M12" s="73"/>
       <c r="N12" s="6">
         <f t="shared" ref="N12:N13" si="2">L12/(K$11+K$13)</f>
         <v>0.21818181818181817</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="2">
         <f>D13</f>
         <v>7277</v>
@@ -1412,21 +1448,21 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53" t="s">
+      <c r="D15" s="71"/>
+      <c r="E15" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53" t="s">
+      <c r="F15" s="71"/>
+      <c r="G15" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="53"/>
+      <c r="H15" s="71"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="2"/>
@@ -1436,7 +1472,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="51"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="10" t="s">
         <v>22</v>
       </c>
@@ -1579,30 +1615,30 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47" t="s">
+      <c r="D32" s="72"/>
+      <c r="E32" s="72" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="47"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="47"/>
+      <c r="E33" s="72"/>
       <c r="H33" s="4" t="s">
         <v>24</v>
       </c>
@@ -1617,22 +1653,22 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="47">
+      <c r="C34" s="72">
         <f>C35+D35</f>
         <v>6548</v>
       </c>
-      <c r="D34" s="47"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="2">
         <f>E35</f>
         <v>7277</v>
       </c>
-      <c r="H34" s="47" t="s">
+      <c r="H34" s="72" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="4" t="s">
@@ -1648,8 +1684,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="47"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="72"/>
       <c r="C35" s="2">
         <v>0</v>
       </c>
@@ -1659,7 +1695,7 @@
       <c r="E35" s="2">
         <v>7277</v>
       </c>
-      <c r="H35" s="47"/>
+      <c r="H35" s="72"/>
       <c r="I35" s="4" t="s">
         <v>20</v>
       </c>
@@ -1673,20 +1709,20 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="47" t="s">
+      <c r="A36" s="72"/>
+      <c r="B36" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="49">
+      <c r="C36" s="73">
         <f>C37+D37</f>
         <v>0.47363471971066906</v>
       </c>
-      <c r="D36" s="49"/>
+      <c r="D36" s="73"/>
       <c r="E36" s="6">
         <f>E37</f>
         <v>0.52636528028933094</v>
       </c>
-      <c r="H36" s="47"/>
+      <c r="H36" s="72"/>
       <c r="I36" s="4" t="s">
         <v>8</v>
       </c>
@@ -1700,8 +1736,8 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="6">
         <f>C35/($C34+$E34)</f>
         <v>0</v>
@@ -1714,7 +1750,7 @@
         <f>E35/($C34+$E34)</f>
         <v>0.52636528028933094</v>
       </c>
-      <c r="H37" s="47"/>
+      <c r="H37" s="72"/>
       <c r="I37" s="4" t="s">
         <v>9</v>
       </c>
@@ -1728,22 +1764,22 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C38" s="72">
         <f>C39+D39</f>
         <v>1198</v>
       </c>
-      <c r="D38" s="47"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="2">
         <f>E39</f>
         <v>767</v>
       </c>
-      <c r="H38" s="47" t="s">
+      <c r="H38" s="72" t="s">
         <v>25</v>
       </c>
       <c r="I38" s="4" t="s">
@@ -1759,8 +1795,8 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="72"/>
       <c r="C39" s="2">
         <v>500</v>
       </c>
@@ -1770,7 +1806,7 @@
       <c r="E39" s="2">
         <v>767</v>
       </c>
-      <c r="H39" s="47"/>
+      <c r="H39" s="72"/>
       <c r="I39" s="4" t="s">
         <v>20</v>
       </c>
@@ -1784,20 +1820,20 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="47" t="s">
+      <c r="A40" s="72"/>
+      <c r="B40" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="49">
+      <c r="C40" s="73">
         <f>C41+D41</f>
         <v>0.60966921119592876</v>
       </c>
-      <c r="D40" s="49"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="6">
         <f>E41</f>
         <v>0.39033078880407124</v>
       </c>
-      <c r="H40" s="47"/>
+      <c r="H40" s="72"/>
       <c r="I40" s="4" t="s">
         <v>8</v>
       </c>
@@ -1811,8 +1847,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="72"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="6">
         <f>C39/($C38+$E38)</f>
         <v>0.2544529262086514</v>
@@ -1825,7 +1861,7 @@
         <f>E39/($C38+$E38)</f>
         <v>0.39033078880407124</v>
       </c>
-      <c r="H41" s="47"/>
+      <c r="H41" s="72"/>
       <c r="I41" s="4" t="s">
         <v>9</v>
       </c>
@@ -1839,22 +1875,22 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="47">
+      <c r="C42" s="72">
         <f>C43+D43</f>
         <v>4642</v>
       </c>
-      <c r="D42" s="47"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="2">
         <f>E43</f>
         <v>5038</v>
       </c>
-      <c r="H42" s="47" t="s">
+      <c r="H42" s="72" t="s">
         <v>26</v>
       </c>
       <c r="I42" s="4" t="s">
@@ -1870,8 +1906,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
-      <c r="B43" s="47"/>
+      <c r="A43" s="72"/>
+      <c r="B43" s="72"/>
       <c r="C43" s="2">
         <v>2530</v>
       </c>
@@ -1881,7 +1917,7 @@
       <c r="E43" s="2">
         <v>5038</v>
       </c>
-      <c r="H43" s="47"/>
+      <c r="H43" s="72"/>
       <c r="I43" s="4" t="s">
         <v>20</v>
       </c>
@@ -1895,20 +1931,20 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
-      <c r="B44" s="47" t="s">
+      <c r="A44" s="72"/>
+      <c r="B44" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="49">
+      <c r="C44" s="73">
         <f>C45+D45</f>
         <v>0.4795454545454545</v>
       </c>
-      <c r="D44" s="49"/>
+      <c r="D44" s="73"/>
       <c r="E44" s="6">
         <f>E45</f>
         <v>0.5204545454545455</v>
       </c>
-      <c r="H44" s="47"/>
+      <c r="H44" s="72"/>
       <c r="I44" s="4" t="s">
         <v>8</v>
       </c>
@@ -1922,8 +1958,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
-      <c r="B45" s="47"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="72"/>
       <c r="C45" s="6">
         <f>C43/($C42+$E42)</f>
         <v>0.26136363636363635</v>
@@ -1936,7 +1972,7 @@
         <f>E43/($C42+$E42)</f>
         <v>0.5204545454545455</v>
       </c>
-      <c r="H45" s="47"/>
+      <c r="H45" s="72"/>
       <c r="I45" s="4" t="s">
         <v>9</v>
       </c>
@@ -1951,11 +1987,39 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:D36"/>
     <mergeCell ref="H42:H45"/>
     <mergeCell ref="H34:H37"/>
     <mergeCell ref="A38:A41"/>
@@ -1968,39 +2032,11 @@
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="H38:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2023,21 +2059,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54" t="s">
+      <c r="D1" s="75"/>
+      <c r="E1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54" t="s">
+      <c r="F1" s="75"/>
+      <c r="G1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="54"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="76" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -2066,7 +2102,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="76"/>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -2093,63 +2129,63 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="75">
         <v>0.87</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54">
+      <c r="D4" s="75"/>
+      <c r="E4" s="75">
         <v>0.8</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54">
+      <c r="F4" s="75"/>
+      <c r="G4" s="75">
         <v>0.86</v>
       </c>
-      <c r="H4" s="54"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="76"/>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54" t="s">
+      <c r="D5" s="75"/>
+      <c r="E5" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54" t="s">
+      <c r="F5" s="75"/>
+      <c r="G5" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="54"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="76"/>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54" t="s">
+      <c r="D6" s="75"/>
+      <c r="E6" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54" t="s">
+      <c r="F6" s="75"/>
+      <c r="G6" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="54"/>
+      <c r="H6" s="75"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="76" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -2175,7 +2211,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="76"/>
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -2199,19 +2235,13 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="G4:H4"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A4:A6"/>
@@ -2222,6 +2252,12 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2232,7 +2268,7 @@
   <dimension ref="A1:AO449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,54 +2286,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="63"/>
+      <c r="A1" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="85"/>
     </row>
     <row r="2" spans="1:41" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="56" t="s">
+      <c r="A2" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="56" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="56" t="s">
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="56" t="s">
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="58"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="79"/>
       <c r="R2"/>
       <c r="S2"/>
       <c r="T2"/>
@@ -2324,33 +2360,33 @@
       <c r="AO2"/>
     </row>
     <row r="3" spans="1:41" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="59" t="s">
+      <c r="A3" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="59" t="s">
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="61"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="80" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="82"/>
       <c r="R3"/>
       <c r="S3"/>
       <c r="T3"/>
@@ -2377,8 +2413,8 @@
       <c r="AO3"/>
     </row>
     <row r="4" spans="1:41" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>61</v>
+      <c r="A4" s="47" t="s">
+        <v>60</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>41</v>
@@ -2454,22 +2490,31 @@
       <c r="AO4"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="B5" s="43">
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="C5" s="43">
+        <v>0.83</v>
+      </c>
+      <c r="D5" s="43">
+        <v>0.69</v>
+      </c>
+      <c r="E5" s="57">
+        <v>0.8</v>
+      </c>
       <c r="F5" s="43">
         <v>0.97750000000000004</v>
       </c>
       <c r="G5" s="43">
         <v>0.82</v>
       </c>
-      <c r="H5" s="90">
+      <c r="H5" s="61">
         <v>0.81</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="57">
         <v>0.78</v>
       </c>
       <c r="J5" s="43">
@@ -2490,66 +2535,82 @@
       <c r="O5" s="43">
         <v>0.84</v>
       </c>
-      <c r="P5" s="87">
+      <c r="P5" s="56">
         <v>0.77</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="Q5" s="57">
         <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="89">
+      <c r="B6" s="43">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="C6" s="56">
         <v>0.86</v>
       </c>
       <c r="D6" s="43">
         <v>0.76</v>
       </c>
+      <c r="E6" s="24">
+        <v>0.75</v>
+      </c>
       <c r="F6" s="43">
         <v>0.99670000000000003</v>
       </c>
-      <c r="G6" s="87">
+      <c r="G6" s="56">
         <v>0.86</v>
       </c>
       <c r="H6" s="43">
         <v>0.76</v>
       </c>
+      <c r="I6" s="24">
+        <v>0.75</v>
+      </c>
       <c r="J6" s="43">
         <v>0.99660000000000004</v>
       </c>
-      <c r="K6" s="87">
+      <c r="K6" s="56">
         <v>0.86</v>
       </c>
-      <c r="L6" s="87">
+      <c r="L6" s="56">
         <v>0.76</v>
       </c>
-      <c r="M6" s="24" t="s">
-        <v>53</v>
+      <c r="M6" s="57">
+        <v>0.75</v>
       </c>
       <c r="N6" s="43">
         <v>0.99670000000000003</v>
       </c>
-      <c r="O6" s="87">
+      <c r="O6" s="56">
         <v>0.86</v>
       </c>
       <c r="P6" s="43">
         <v>0.76</v>
       </c>
-      <c r="Q6" s="24" t="s">
-        <v>53</v>
+      <c r="Q6" s="57">
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:41" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
+      <c r="B7" s="44">
+        <v>0.99390000000000001</v>
+      </c>
+      <c r="C7" s="44">
+        <v>0.79</v>
+      </c>
+      <c r="D7" s="67">
+        <v>0.79</v>
+      </c>
+      <c r="E7" s="45">
+        <v>0.73</v>
+      </c>
       <c r="F7" s="44">
         <v>0.99470000000000003</v>
       </c>
@@ -2612,90 +2673,92 @@
       <c r="AO7"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="65"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="88"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="67"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="91"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="84"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="85"/>
+    </row>
+    <row r="11" spans="1:41" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="63"/>
-    </row>
-    <row r="11" spans="1:41" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="56" t="s">
+      <c r="B11" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="56" t="s">
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="58"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" s="78"/>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="79"/>
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -2722,37 +2785,37 @@
       <c r="AO11"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="82"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
         <v>60</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="61"/>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
-        <v>61</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>41</v>
@@ -2804,20 +2867,20 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="49" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="43">
-        <v>0.94669999999999999</v>
-      </c>
-      <c r="C14" s="90">
-        <v>0.87</v>
-      </c>
-      <c r="D14" s="43">
+        <v>0.97250000000000003</v>
+      </c>
+      <c r="C14" s="62">
         <v>0.8</v>
       </c>
-      <c r="E14" s="91">
-        <v>0.86</v>
+      <c r="D14" s="62">
+        <v>0.69</v>
+      </c>
+      <c r="E14" s="64">
+        <v>0.73</v>
       </c>
       <c r="F14" s="43">
         <v>0.98170000000000002</v>
@@ -2825,7 +2888,7 @@
       <c r="G14" s="43">
         <v>0.81</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="56">
         <v>0.76</v>
       </c>
       <c r="I14" s="24">
@@ -2834,75 +2897,97 @@
       <c r="J14" s="43">
         <v>0.98650000000000004</v>
       </c>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
+      <c r="K14" s="43">
+        <v>0.79</v>
+      </c>
+      <c r="L14" s="43">
+        <v>0.61</v>
+      </c>
+      <c r="M14" s="24">
+        <v>0.71</v>
+      </c>
+      <c r="N14" s="43">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="O14" s="43">
+        <v>0.82</v>
+      </c>
+      <c r="P14" s="43">
+        <v>0.72</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="49" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="43">
-        <v>0.99680000000000002</v>
-      </c>
-      <c r="C15" s="43">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="C15" s="56">
         <v>0.85</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="56">
         <v>0.74</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="57">
         <v>0.78</v>
       </c>
       <c r="F15" s="43">
         <v>0.99580000000000002</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="56">
         <v>0.85</v>
       </c>
       <c r="H15" s="43">
         <v>0.74</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="57">
         <v>0.78</v>
       </c>
       <c r="J15" s="43">
         <v>0.99580000000000002</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="56">
         <v>0.85</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="56">
         <v>0.74</v>
       </c>
-      <c r="M15" s="88">
+      <c r="M15" s="57">
         <v>0.78</v>
       </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43">
+      <c r="N15" s="43">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="O15" s="56">
         <v>0.85</v>
       </c>
-      <c r="P15" s="43">
+      <c r="P15" s="56">
         <v>0.74</v>
       </c>
-      <c r="Q15" s="88">
+      <c r="Q15" s="57">
         <v>0.78</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="72" t="s">
+      <c r="A16" s="50" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="44">
-        <v>0.98860000000000003</v>
-      </c>
-      <c r="C16" s="44">
-        <v>0.78</v>
-      </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="45"/>
+        <v>0.99450000000000005</v>
+      </c>
+      <c r="C16" s="65">
+        <v>0.76</v>
+      </c>
+      <c r="D16" s="65">
+        <v>0.66</v>
+      </c>
+      <c r="E16" s="66">
+        <v>0.73</v>
+      </c>
       <c r="F16" s="44">
         <v>0.99650000000000005</v>
       </c>
@@ -2918,13 +3003,27 @@
       <c r="J16" s="44">
         <v>0.99970000000000003</v>
       </c>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="45"/>
+      <c r="K16" s="44">
+        <v>0.79</v>
+      </c>
+      <c r="L16" s="44">
+        <v>0.63</v>
+      </c>
+      <c r="M16" s="45">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N16" s="44">
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="O16" s="44">
+        <v>0.81</v>
+      </c>
+      <c r="P16" s="44">
+        <v>0.73</v>
+      </c>
+      <c r="Q16" s="45">
+        <v>0.69</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17"/>
@@ -2965,11 +3064,15 @@
       <c r="Q18"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
+      <c r="A19" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="79"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
@@ -2984,11 +3087,15 @@
       <c r="Q19"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
+      <c r="A20" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20"/>
@@ -3003,11 +3110,21 @@
       <c r="Q20"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
+      <c r="A21" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
@@ -3022,11 +3139,21 @@
       <c r="Q21"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
+      <c r="A22" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="43">
+        <v>0.94669999999999999</v>
+      </c>
+      <c r="C22" s="61">
+        <v>0.87</v>
+      </c>
+      <c r="D22" s="62">
+        <v>0.8</v>
+      </c>
+      <c r="E22" s="63">
+        <v>0.86</v>
+      </c>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
@@ -3041,11 +3168,16 @@
       <c r="Q22"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="A23" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="43">
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="C23" s="43">
+        <v>0.85</v>
+      </c>
+      <c r="D23" s="43"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
@@ -3060,11 +3192,17 @@
       <c r="Q23"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
+      <c r="A24" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="44">
+        <v>0.98860000000000003</v>
+      </c>
+      <c r="C24" s="44">
+        <v>0.78</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24"/>
@@ -11154,13 +11292,9 @@
       <c r="Q449"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A10:Q10"/>
+  <mergeCells count="20">
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A8:Q9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:M12"/>
     <mergeCell ref="N12:Q12"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="J3:M3"/>
@@ -11174,6 +11308,11 @@
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A10:Q10"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11182,10 +11321,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11204,26 +11343,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77"/>
+      <c r="A1" s="53"/>
       <c r="B1" s="20"/>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="78" t="s">
+      <c r="D1" s="93"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="78" t="s">
+      <c r="G1" s="93"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="79"/>
-      <c r="K1" s="80"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="94"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="95" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -11261,7 +11400,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="18" t="s">
         <v>49</v>
       </c>
@@ -11272,7 +11411,7 @@
         <v>0.58468750000000003</v>
       </c>
       <c r="E3" s="27">
-        <f t="shared" ref="E3:E17" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E19" si="0">D3-C3</f>
         <v>5.7685185185185284E-2</v>
       </c>
       <c r="F3" s="28">
@@ -11282,7 +11421,7 @@
         <v>0.59534722222222225</v>
       </c>
       <c r="H3" s="27">
-        <f t="shared" ref="H3:H17" si="1">G3-F3</f>
+        <f t="shared" ref="H3:H16" si="1">G3-F3</f>
         <v>3.5185185185185874E-3</v>
       </c>
       <c r="I3" s="28">
@@ -11292,12 +11431,12 @@
         <v>0.59592592592592586</v>
       </c>
       <c r="K3" s="27">
-        <f t="shared" ref="K3:K17" si="2">J3-I3</f>
+        <f t="shared" ref="K3:K19" si="2">J3-I3</f>
         <v>9.2592592592533052E-5</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="82"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="18" t="s">
         <v>50</v>
       </c>
@@ -11333,7 +11472,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="18" t="s">
         <v>51</v>
       </c>
@@ -11369,7 +11508,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="18" t="s">
         <v>52</v>
       </c>
@@ -11390,7 +11529,7 @@
         <v>0.51623842592592595</v>
       </c>
       <c r="H6" s="27">
-        <f t="shared" si="1"/>
+        <f>G6-F6</f>
         <v>3.263888888888955E-3</v>
       </c>
       <c r="I6" s="28">
@@ -11405,275 +11544,451 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="82"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="C7" s="28">
+        <v>1.0069444444444444E-3</v>
+      </c>
+      <c r="D7" s="29">
+        <v>6.6805555555555562E-2</v>
+      </c>
+      <c r="E7" s="27">
+        <f t="shared" si="0"/>
+        <v>6.5798611111111113E-2</v>
+      </c>
+      <c r="F7" s="28">
+        <v>7.4201388888888886E-2</v>
+      </c>
+      <c r="G7" s="29">
+        <v>7.7557870370370374E-2</v>
+      </c>
+      <c r="H7" s="27">
+        <f>G7-F7</f>
+        <v>3.3564814814814881E-3</v>
+      </c>
+      <c r="I7" s="28">
+        <v>7.9895833333333333E-2</v>
+      </c>
+      <c r="J7" s="29">
+        <v>8.1469907407407408E-2</v>
+      </c>
+      <c r="K7" s="27">
+        <f t="shared" si="2"/>
+        <v>1.574074074074075E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
-      <c r="E8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="K8" s="27"/>
+      <c r="A8" s="96"/>
+      <c r="B8" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0.91982638888888879</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0.98322916666666671</v>
+      </c>
+      <c r="E8" s="27">
+        <f t="shared" si="0"/>
+        <v>6.3402777777777919E-2</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0.99003472222222222</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0.99326388888888895</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" ref="H8:H9" si="3">G8-F8</f>
+        <v>3.2291666666667274E-3</v>
+      </c>
+      <c r="I8" s="28">
+        <v>0.99685185185185177</v>
+      </c>
+      <c r="J8" s="29">
+        <v>0.9986342592592593</v>
+      </c>
+      <c r="K8" s="27">
+        <f t="shared" si="2"/>
+        <v>1.782407407407538E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="35">
-        <f>AVERAGE(E2:E8)</f>
-        <v>5.0590277777777783E-2</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="35">
-        <f>AVERAGE(H2:H8)</f>
-        <v>3.3379629629629757E-3</v>
-      </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="35">
-        <f>AVERAGE(K2:K8)</f>
-        <v>1.2962962962962648E-3</v>
+      <c r="A9" s="96"/>
+      <c r="B9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0.48791666666666672</v>
+      </c>
+      <c r="E9" s="27">
+        <f t="shared" si="0"/>
+        <v>4.3472222222222301E-2</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0.49436342592592591</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0.49793981481481481</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="3"/>
+        <v>3.5763888888888928E-3</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0.50236111111111115</v>
+      </c>
+      <c r="J9" s="29">
+        <v>0.50482638888888887</v>
+      </c>
+      <c r="K9" s="27">
+        <f t="shared" si="2"/>
+        <v>2.4652777777777191E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="E10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="84" t="s">
+      <c r="A10" s="96"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="35">
+        <f>AVERAGE(E2:E9)</f>
+        <v>5.3203125000000032E-2</v>
+      </c>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="35">
+        <f>AVERAGE(H2:H9)</f>
+        <v>3.3564814814814985E-3</v>
+      </c>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="35">
+        <f>AVERAGE(K2:K9)</f>
+        <v>1.537905092592582E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="54"/>
+      <c r="E11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B12" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C12" s="38">
         <v>5.2199074074074066E-3</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D12" s="39">
         <v>8.5995370370370357E-3</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E12" s="34">
         <f t="shared" si="0"/>
         <v>3.3796296296296291E-3</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F12" s="38">
         <v>5.7905092592592598E-2</v>
       </c>
-      <c r="G11" s="39">
+      <c r="G12" s="39">
         <v>6.4386574074074068E-2</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H12" s="34">
         <f t="shared" si="1"/>
         <v>6.48148148148147E-3</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I12" s="38">
         <v>6.8310185185185182E-2</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J12" s="39">
         <v>7.0856481481481479E-2</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K12" s="34">
         <f t="shared" si="2"/>
         <v>2.5462962962962965E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="85"/>
-      <c r="B12" s="18" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="98"/>
+      <c r="B13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C13" s="28">
         <v>0.52023148148148146</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D13" s="29">
         <v>0.52510416666666659</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E13" s="27">
         <f t="shared" si="0"/>
         <v>4.8726851851851327E-3</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F13" s="28">
         <v>0.58479166666666671</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G13" s="29">
         <v>0.59159722222222222</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H13" s="27">
         <f t="shared" si="1"/>
         <v>6.8055555555555092E-3</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I13" s="28">
         <v>0.59539351851851852</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J13" s="29">
         <v>0.59577546296296291</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K13" s="27">
         <f t="shared" si="2"/>
         <v>3.8194444444439313E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="85"/>
-      <c r="B13" s="18" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="98"/>
+      <c r="B14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C14" s="28">
         <v>0.64236111111111105</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D14" s="29">
         <v>0.6461689814814815</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E14" s="27">
         <f t="shared" si="0"/>
         <v>3.8078703703704475E-3</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F14" s="28">
         <v>0.68982638888888881</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G14" s="29">
         <v>0.69658564814814816</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H14" s="27">
         <f t="shared" si="1"/>
         <v>6.7592592592593537E-3</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I14" s="28">
         <v>0.70034722222222223</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J14" s="29">
         <v>0.70526620370370363</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K14" s="27">
         <f t="shared" si="2"/>
         <v>4.9189814814813992E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="85"/>
-      <c r="B14" s="18" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="98"/>
+      <c r="B15" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C15" s="28">
         <v>0.53849537037037043</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D15" s="29">
         <v>0.54150462962962964</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E15" s="27">
         <f t="shared" si="0"/>
         <v>3.0092592592592116E-3</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F15" s="28">
         <v>0.58422453703703703</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G15" s="29">
         <v>0.5896527777777778</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H15" s="27">
         <f t="shared" si="1"/>
         <v>5.4282407407407751E-3</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I15" s="28">
         <v>0.59320601851851851</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J15" s="29">
         <v>0.59619212962962964</v>
       </c>
-      <c r="K14" s="27">
-        <f>J14-I14</f>
+      <c r="K15" s="27">
+        <f>J15-I15</f>
         <v>2.9861111111111338E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="85"/>
-      <c r="B15" s="18" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="98"/>
+      <c r="B16" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C16" s="28">
         <v>0.43476851851851855</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D16" s="29">
         <v>0.43965277777777773</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E16" s="27">
         <f t="shared" si="0"/>
         <v>4.8842592592591716E-3</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F16" s="28">
         <v>0.50653935185185184</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G16" s="29">
         <v>0.51217592592592587</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H16" s="27">
         <f t="shared" si="1"/>
         <v>5.63657407407403E-3</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I16" s="28">
         <v>0.51634259259259263</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J16" s="29">
         <v>0.51678240740740744</v>
       </c>
-      <c r="K15" s="27">
+      <c r="K16" s="27">
         <f t="shared" si="2"/>
         <v>4.3981481481480955E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
-      <c r="B16" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="K16" s="27"/>
-    </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
-      <c r="E17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="K17" s="27"/>
-    </row>
-    <row r="18" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="86"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42">
-        <f>AVERAGE(E11:E17)</f>
-        <v>3.9907407407407183E-3</v>
-      </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="42">
-        <f>AVERAGE(H11:H17)</f>
-        <v>6.2222222222222279E-3</v>
-      </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42">
-        <f>AVERAGE(K11:K17)</f>
-        <v>2.2546296296296064E-3</v>
+      <c r="A17" s="98"/>
+      <c r="B17" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0.99383101851851852</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0.99880787037037033</v>
+      </c>
+      <c r="E17" s="27">
+        <f t="shared" si="0"/>
+        <v>4.9768518518518157E-3</v>
+      </c>
+      <c r="F17" s="28">
+        <v>6.6909722222222232E-2</v>
+      </c>
+      <c r="G17" s="29">
+        <v>7.3599537037037033E-2</v>
+      </c>
+      <c r="H17" s="27">
+        <f>G17-F17</f>
+        <v>6.6898148148148012E-3</v>
+      </c>
+      <c r="I17" s="28">
+        <v>7.7662037037037043E-2</v>
+      </c>
+      <c r="J17" s="29">
+        <v>7.9687500000000008E-2</v>
+      </c>
+      <c r="K17" s="27">
+        <f t="shared" si="2"/>
+        <v>2.025462962962965E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="98"/>
+      <c r="B18" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="28">
+        <v>0.91289351851851863</v>
+      </c>
+      <c r="D18" s="29">
+        <v>0.91748842592592583</v>
+      </c>
+      <c r="E18" s="27">
+        <f t="shared" si="0"/>
+        <v>4.5949074074072005E-3</v>
+      </c>
+      <c r="F18" s="28">
+        <v>0.98340277777777774</v>
+      </c>
+      <c r="G18" s="29">
+        <v>0.98934027777777767</v>
+      </c>
+      <c r="H18" s="27">
+        <f t="shared" ref="H18:H19" si="4">G18-F18</f>
+        <v>5.9374999999999289E-3</v>
+      </c>
+      <c r="I18" s="28">
+        <v>0.99341435185185178</v>
+      </c>
+      <c r="J18" s="29">
+        <v>0.99649305555555545</v>
+      </c>
+      <c r="K18" s="27">
+        <f t="shared" si="2"/>
+        <v>3.0787037037036669E-3</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="K19" s="27"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="A19" s="98"/>
+      <c r="B19" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="28">
+        <v>0.43958333333333338</v>
+      </c>
+      <c r="D19" s="29">
+        <v>0.44283564814814813</v>
+      </c>
+      <c r="E19" s="27">
+        <f t="shared" si="0"/>
+        <v>3.2523148148147496E-3</v>
+      </c>
+      <c r="F19" s="28">
+        <v>0.48796296296296293</v>
+      </c>
+      <c r="G19" s="29">
+        <v>0.49414351851851851</v>
+      </c>
+      <c r="H19" s="27">
+        <f t="shared" si="4"/>
+        <v>6.180555555555578E-3</v>
+      </c>
+      <c r="I19" s="28">
+        <v>0.49797453703703703</v>
+      </c>
+      <c r="J19" s="29">
+        <v>0.50222222222222224</v>
+      </c>
+      <c r="K19" s="27">
+        <f t="shared" si="2"/>
+        <v>4.2476851851852016E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="55"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42">
+        <f>AVERAGE(E12:E19)</f>
+        <v>4.0972222222221697E-3</v>
+      </c>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="42">
+        <f>AVERAGE(H12:H19)</f>
+        <v>6.2398726851851808E-3</v>
+      </c>
+      <c r="I20" s="40"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42">
+        <f>AVERAGE(K12:K19)</f>
+        <v>2.5781249999999832E-3</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E21" s="27"/>
@@ -11683,48 +11998,98 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E22" s="27"/>
       <c r="H22" s="27"/>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="K23" s="27"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="27"/>
+      <c r="H24" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:E2 E3:E22">
-    <cfRule type="timePeriod" dxfId="13" priority="7" timePeriod="lastWeek">
+  <conditionalFormatting sqref="C2:E2 E3:E24">
+    <cfRule type="timePeriod" dxfId="14" priority="15" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(C2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(C2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8 H10:H17 H19:H22">
-    <cfRule type="timePeriod" dxfId="12" priority="6" timePeriod="lastWeek">
+  <conditionalFormatting sqref="H21:H24 H2:H7 H11:H17">
+    <cfRule type="timePeriod" dxfId="13" priority="14" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(H2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K8 K10:K17 K19:K21">
-    <cfRule type="timePeriod" dxfId="11" priority="5" timePeriod="lastWeek">
+  <conditionalFormatting sqref="K21:K23 K2:K7 K11:K17">
+    <cfRule type="timePeriod" dxfId="12" priority="13" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(K2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="timePeriod" dxfId="11" priority="12" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(H10,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H10,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="timePeriod" dxfId="10" priority="11" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(K10,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K10,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(H20,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H20,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="timePeriod" dxfId="8" priority="9" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(K20,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K20,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="timePeriod" dxfId="7" priority="8" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(H18,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H18,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="timePeriod" dxfId="6" priority="7" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(H19,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H19,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="timePeriod" dxfId="5" priority="6" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(K18,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K18,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="timePeriod" dxfId="4" priority="5" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(K19,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K19,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="timePeriod" dxfId="3" priority="4" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(H8,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H8,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="timePeriod" dxfId="10" priority="4" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(H9,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H9,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="timePeriod" dxfId="9" priority="3" timePeriod="lastWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(K9,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K9,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(K8,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K8,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="timePeriod" dxfId="8" priority="2" timePeriod="lastWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(H18,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(H18,0)&lt;(WEEKDAY(TODAY())+7))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="timePeriod" dxfId="7" priority="1" timePeriod="lastWeek">
-      <formula>AND(TODAY()-ROUNDDOWN(K18,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K18,0)&lt;(WEEKDAY(TODAY())+7))</formula>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
+      <formula>AND(TODAY()-ROUNDDOWN(K9,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K9,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>